<commit_message>
Python has another ramp
</commit_message>
<xml_diff>
--- a/Documents/MapAnalysis.xlsx
+++ b/Documents/MapAnalysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -70,13 +70,16 @@
   </si>
   <si>
     <t>1 Ramp</t>
+  </si>
+  <si>
+    <t>1 Ramp 1 Wide Ramp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +95,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +128,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -253,10 +268,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -297,8 +313,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,7 +626,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,14 +748,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>